<commit_message>
Updating training and removing old files to prep for final training
</commit_message>
<xml_diff>
--- a/Tracking Hemo Scores.xlsx
+++ b/Tracking Hemo Scores.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josie/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josie/PycharmProjects/HemoPheno4HF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A30431-4444-0942-B73F-CD3833D0A893}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B10F71A-9E20-6D40-A47C-3FE3BCB72EAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2460" windowWidth="27200" windowHeight="14860" activeTab="2" xr2:uid="{D6E5111C-8D9C-F44B-AF27-7E99F01D8FA2}"/>
+    <workbookView xWindow="3900" yWindow="2460" windowWidth="27200" windowHeight="14860" activeTab="3" xr2:uid="{D6E5111C-8D9C-F44B-AF27-7E99F01D8FA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Clustering" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId4"/>
+    <sheet name="Model Training" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="107">
   <si>
     <t>Dataset = Hemo</t>
   </si>
@@ -352,6 +353,12 @@
   </si>
   <si>
     <t>Clustering Method</t>
+  </si>
+  <si>
+    <t>Training Params</t>
+  </si>
+  <si>
+    <t>Ward clustering</t>
   </si>
 </sst>
 </file>
@@ -455,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,6 +488,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -813,7 +823,7 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1319,28 +1329,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="23" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="26"/>
     </row>
     <row r="2" spans="1:19">
       <c r="B2" s="5" t="s">
@@ -1822,11 +1832,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD97EBB-582D-1C42-8D6C-41E4A2B95EB5}">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+    <sheetView zoomScale="189" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1835,22 +1845,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
@@ -2241,7 +2251,276 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3866840-864A-3F42-9D0E-5659E519615F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA91C14-FFE7-9F45-ACFD-ECAA102128FB}">
+  <dimension ref="A1:S9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="189" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="B1" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="B2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="6"/>
+      <c r="P2" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="6"/>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="10"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="10"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+    </row>
+    <row r="7" spans="1:19" s="21" customFormat="1">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="10"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="10"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC4D4C0E-ED39-DC48-91B0-FE8C4A6E9DB2}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>